<commit_message>
corrected skiing excel file rip
</commit_message>
<xml_diff>
--- a/skiing_dist.xlsx
+++ b/skiing_dist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathancarlson/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathancarlson/Desktop/programs/MATH 532/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3449A893-38ED-6E46-8773-F8762BCA38D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6EEEDC-8C22-C645-8343-CAA8CE5E1EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="660" windowWidth="28040" windowHeight="17160" xr2:uid="{347E3398-47C5-124E-A0C4-26C16EA01850}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J10"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,7 +497,7 @@
         <v>66</v>
       </c>
       <c r="I2">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J2">
         <v>161</v>

</xml_diff>